<commit_message>
Actualizacion de Practica4 , es la Nueva
</commit_message>
<xml_diff>
--- a/Practica 4/AFD.xlsx
+++ b/Practica 4/AFD.xlsx
@@ -2,27 +2,32 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Escom4sem\TeoriaComputacional\Tareas\Practica4\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="594" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="594" firstSheet="6" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
-    <sheet name="Hoja4" sheetId="6" r:id="rId4"/>
+    <sheet name="SheetResultadosAutomata" sheetId="3" r:id="rId3"/>
+    <sheet name="SheetResultadosAutomata1" sheetId="4" r:id="rId4"/>
+    <sheet name="Hoja3" sheetId="5" r:id="rId5"/>
+    <sheet name="SheetResultadosAutomata2" sheetId="6" r:id="rId6"/>
+    <sheet name="Hoja5" sheetId="7" r:id="rId7"/>
+    <sheet name="SheetResultadosAutomata3" sheetId="8" r:id="rId8"/>
+    <sheet name="Hoja4" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="24">
   <si>
     <t>δ</t>
   </si>
@@ -51,12 +56,12 @@
     <t>q0</t>
   </si>
   <si>
+    <t>a</t>
+  </si>
+  <si>
     <t>→p</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
     <t>q</t>
   </si>
   <si>
@@ -72,10 +77,28 @@
     <t>u</t>
   </si>
   <si>
+    <t>*u</t>
+  </si>
+  <si>
     <t>p</t>
   </si>
   <si>
-    <t>*u</t>
+    <t>→q0,q3</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>q2,q4</t>
+  </si>
+  <si>
+    <t>*q3,q1</t>
+  </si>
+  <si>
+    <t>→q0,q2</t>
+  </si>
+  <si>
+    <t>*q3</t>
   </si>
 </sst>
 </file>
@@ -137,7 +160,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -429,7 +452,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,7 +525,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360"/>
 </worksheet>
 </file>
 
@@ -521,12 +544,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>11</v>
@@ -566,19 +589,136 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -587,16 +727,16 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>11</v>
@@ -636,23 +776,83 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,11 +861,11 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>1</v>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -673,43 +873,150 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
       </c>
     </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
         <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -717,10 +1024,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>